<commit_message>
New Inpiut data 1
</commit_message>
<xml_diff>
--- a/Sathapna/Input_Data/Inputs.xlsx
+++ b/Sathapna/Input_Data/Inputs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="911" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="911" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Valid Login" sheetId="1" state="visible" r:id="rId2"/>
@@ -53,10 +53,10 @@
     <t>User id</t>
   </si>
   <si>
-    <t>RamMadhav7</t>
-  </si>
-  <si>
-    <t>Ram7</t>
+    <t>RamMadhav8</t>
+  </si>
+  <si>
+    <t>Ram8</t>
   </si>
   <si>
     <t>Mobilenumber</t>
@@ -77,7 +77,7 @@
     <t>companyname</t>
   </si>
   <si>
-    <t>DMTraders27</t>
+    <t>DMTraders28</t>
   </si>
   <si>
     <t>mobilenum</t>
@@ -119,7 +119,7 @@
     <t>username</t>
   </si>
   <si>
-    <t>User27</t>
+    <t>User28</t>
   </si>
   <si>
     <t>roleid</t>
@@ -471,7 +471,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -494,7 +494,7 @@
         <v>61</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>17027</v>
+        <v>17028</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -523,7 +523,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -812,7 +812,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -851,7 +851,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>9916560546</v>
+        <v>9916560548</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -880,8 +880,8 @@
   </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -904,7 +904,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>17027</v>
+        <v>17028</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -928,7 +928,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>9916569249</v>
+        <v>9916569247</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -936,7 +936,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>17027</v>
+        <v>17028</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -974,7 +974,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -997,7 +997,7 @@
         <v>21</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>17027</v>
+        <v>17028</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1066,7 +1066,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>17027</v>
+        <v>17028</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1074,7 +1074,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>3327</v>
+        <v>3328</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1090,7 +1090,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>991656924824</v>
+        <v>991656924825</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1151,7 +1151,7 @@
         <v>21</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>17027</v>
+        <v>17028</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1341,7 +1341,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1364,7 +1364,7 @@
         <v>54</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>17027</v>
+        <v>17028</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1372,7 +1372,7 @@
         <v>55</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>3327</v>
+        <v>3328</v>
       </c>
     </row>
   </sheetData>
@@ -1394,7 +1394,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1417,7 +1417,7 @@
         <v>56</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>17027</v>
+        <v>17028</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>